<commit_message>
data finished for magneto resistance
</commit_message>
<xml_diff>
--- a/Data/Magneto resistance/Magneto resistance .xlsx
+++ b/Data/Magneto resistance/Magneto resistance .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16520" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>V5</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">probe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">error on input current </t>
+  </si>
+  <si>
+    <t>98.7.988</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -208,13 +214,152 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="211">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -251,6 +396,75 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -287,6 +501,75 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -616,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K61"/>
+  <dimension ref="A3:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -628,9 +911,10 @@
     <col min="2" max="2" width="23.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -652,8 +936,11 @@
       <c r="G3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>1.7</v>
       </c>
@@ -675,8 +962,11 @@
       <c r="G4">
         <v>3.0170625891201001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>3.4</v>
       </c>
@@ -699,7 +989,7 @@
         <v>3.2423536424725445E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5.0999999999999996</v>
       </c>
@@ -722,7 +1012,7 @@
         <v>2.1817014985032444E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6.8</v>
       </c>
@@ -745,52 +1035,142 @@
         <v>6.0249481325564305E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>8.5</v>
       </c>
       <c r="B8">
-        <v>105.77499999999999</v>
+        <v>130.71666666666667</v>
       </c>
       <c r="C8">
-        <v>1.2750222814452383</v>
+        <v>1.1637192205349305</v>
       </c>
       <c r="D8">
-        <v>67.624142857142857</v>
+        <v>68.114000000000004</v>
       </c>
       <c r="E8">
-        <v>4.4126441700446779E-2</v>
+        <v>6.1035508790648764E-2</v>
       </c>
       <c r="F8">
-        <v>97.77285714285712</v>
+        <v>98.213999999999999</v>
       </c>
       <c r="G8">
-        <v>5.4379618030494722E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>3.824561769310663E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="B9" s="3">
+        <v>159.5</v>
+      </c>
+      <c r="C9">
+        <v>3.5547663265485729</v>
+      </c>
+      <c r="D9">
+        <v>68.650000000000006</v>
+      </c>
+      <c r="E9">
+        <v>5.4772255750521283E-2</v>
+      </c>
+      <c r="F9">
+        <v>98.721000000000004</v>
+      </c>
+      <c r="G9">
+        <v>4.4350873723069874E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="B10">
+        <v>187.36666666666667</v>
+      </c>
+      <c r="C10">
+        <v>1.3832329280830946</v>
+      </c>
+      <c r="D10">
+        <v>69.270799999999994</v>
+      </c>
+      <c r="E10">
+        <v>7.1006728945610886E-2</v>
+      </c>
+      <c r="F10">
+        <v>99.363749999999982</v>
+      </c>
+      <c r="G10">
+        <v>5.2898150116185635E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>13.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="B11">
+        <v>213.25</v>
+      </c>
+      <c r="C11">
+        <v>4.4949466575862109</v>
+      </c>
+      <c r="D11">
+        <v>69.816666666666677</v>
+      </c>
+      <c r="E11">
+        <v>7.527726527091011E-2</v>
+      </c>
+      <c r="F11">
+        <v>99.951666666666668</v>
+      </c>
+      <c r="G11">
+        <v>5.6715665090576461E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="B12">
+        <v>238.91666666666666</v>
+      </c>
+      <c r="C12">
+        <v>4.3995523188229742</v>
+      </c>
+      <c r="D12">
+        <v>70.51766666666667</v>
+      </c>
+      <c r="E12">
+        <v>6.7417109598876965E-2</v>
+      </c>
+      <c r="F12">
+        <v>100.60454545454546</v>
+      </c>
+      <c r="G12">
+        <v>7.0484556657986142E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>266.41666666666669</v>
+      </c>
+      <c r="C13">
+        <v>6.4590786471211965</v>
+      </c>
+      <c r="D13">
+        <v>71.141545454545451</v>
+      </c>
+      <c r="E13">
+        <v>8.5675391608516865E-2</v>
+      </c>
+      <c r="F13">
+        <v>101.354</v>
+      </c>
+      <c r="G13">
+        <v>8.7284591996526703E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -844,6 +1224,21 @@
       <c r="F20" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="B21">
@@ -859,7 +1254,22 @@
         <v>104</v>
       </c>
       <c r="F21">
-        <v>107.4</v>
+        <v>129.5</v>
+      </c>
+      <c r="G21">
+        <v>158</v>
+      </c>
+      <c r="H21">
+        <v>187.6</v>
+      </c>
+      <c r="I21">
+        <v>206</v>
+      </c>
+      <c r="J21">
+        <v>236</v>
+      </c>
+      <c r="K21">
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -876,7 +1286,22 @@
         <v>107</v>
       </c>
       <c r="F22">
-        <v>104</v>
+        <v>129.1</v>
+      </c>
+      <c r="G22">
+        <v>159</v>
+      </c>
+      <c r="H22">
+        <v>187.5</v>
+      </c>
+      <c r="I22">
+        <v>217</v>
+      </c>
+      <c r="J22">
+        <v>240</v>
+      </c>
+      <c r="K22">
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -893,7 +1318,22 @@
         <v>104</v>
       </c>
       <c r="F23">
-        <v>106</v>
+        <v>130</v>
+      </c>
+      <c r="G23">
+        <v>158</v>
+      </c>
+      <c r="H23">
+        <v>187.7</v>
+      </c>
+      <c r="I23">
+        <v>208</v>
+      </c>
+      <c r="J23">
+        <v>239</v>
+      </c>
+      <c r="K23">
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -910,7 +1350,22 @@
         <v>107</v>
       </c>
       <c r="F24">
-        <v>105.7</v>
+        <v>132</v>
+      </c>
+      <c r="G24">
+        <v>159</v>
+      </c>
+      <c r="H24">
+        <v>188.6</v>
+      </c>
+      <c r="I24">
+        <v>217</v>
+      </c>
+      <c r="J24">
+        <v>240</v>
+      </c>
+      <c r="K24">
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -927,7 +1382,22 @@
         <v>106</v>
       </c>
       <c r="F25">
-        <v>106</v>
+        <v>130</v>
+      </c>
+      <c r="G25">
+        <v>160</v>
+      </c>
+      <c r="H25">
+        <v>186</v>
+      </c>
+      <c r="I25">
+        <v>218</v>
+      </c>
+      <c r="J25">
+        <v>237</v>
+      </c>
+      <c r="K25">
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -944,7 +1414,22 @@
         <v>106</v>
       </c>
       <c r="F26">
-        <v>107.2</v>
+        <v>132</v>
+      </c>
+      <c r="G26">
+        <v>161</v>
+      </c>
+      <c r="H26">
+        <v>187</v>
+      </c>
+      <c r="I26">
+        <v>208</v>
+      </c>
+      <c r="J26">
+        <v>241</v>
+      </c>
+      <c r="K26">
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -961,7 +1446,22 @@
         <v>104</v>
       </c>
       <c r="F27">
-        <v>104</v>
+        <v>130</v>
+      </c>
+      <c r="G27">
+        <v>156</v>
+      </c>
+      <c r="H27">
+        <v>188</v>
+      </c>
+      <c r="I27">
+        <v>217</v>
+      </c>
+      <c r="J27">
+        <v>234</v>
+      </c>
+      <c r="K27">
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -978,7 +1478,22 @@
         <v>107</v>
       </c>
       <c r="F28">
-        <v>107</v>
+        <v>130</v>
+      </c>
+      <c r="G28">
+        <v>155</v>
+      </c>
+      <c r="H28">
+        <v>188</v>
+      </c>
+      <c r="I28">
+        <v>208</v>
+      </c>
+      <c r="J28">
+        <v>244</v>
+      </c>
+      <c r="K28">
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -995,7 +1510,22 @@
         <v>107</v>
       </c>
       <c r="F29">
-        <v>104</v>
+        <v>132</v>
+      </c>
+      <c r="G29">
+        <v>162</v>
+      </c>
+      <c r="H29">
+        <v>189</v>
+      </c>
+      <c r="I29">
+        <v>217</v>
+      </c>
+      <c r="J29">
+        <v>233</v>
+      </c>
+      <c r="K29">
+        <v>274</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1016,7 +1546,22 @@
         <v>104</v>
       </c>
       <c r="F30">
-        <v>107</v>
+        <v>130</v>
+      </c>
+      <c r="G30">
+        <v>155</v>
+      </c>
+      <c r="H30">
+        <v>185</v>
+      </c>
+      <c r="I30">
+        <v>216</v>
+      </c>
+      <c r="J30">
+        <v>245</v>
+      </c>
+      <c r="K30">
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1037,7 +1582,22 @@
         <v>106</v>
       </c>
       <c r="F31">
-        <v>106</v>
+        <v>132</v>
+      </c>
+      <c r="G31">
+        <v>165</v>
+      </c>
+      <c r="H31">
+        <v>185</v>
+      </c>
+      <c r="I31">
+        <v>214</v>
+      </c>
+      <c r="J31">
+        <v>233</v>
+      </c>
+      <c r="K31">
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1057,10 +1617,25 @@
         <v>104.598</v>
       </c>
       <c r="F32">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>132</v>
+      </c>
+      <c r="G32">
+        <v>166</v>
+      </c>
+      <c r="H32">
+        <v>189</v>
+      </c>
+      <c r="I32">
+        <v>213</v>
+      </c>
+      <c r="J32">
+        <v>245</v>
+      </c>
+      <c r="K32">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="C33" s="1">
         <f>_xlfn.STDEV.S(C21:C32)</f>
         <v>2.1430031745334879</v>
@@ -1072,11 +1647,31 @@
         <v>107.6</v>
       </c>
       <c r="F33" s="1">
-        <f>_xlfn.STDEV.S(F21:F32)</f>
-        <v>1.2750222814452383</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <f t="shared" ref="F33:K33" si="0">_xlfn.STDEV.S(F21:F32)</f>
+        <v>1.1637192205349305</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5547663265485729</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3832329280830946</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4949466575862109</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3995523188229742</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="0"/>
+        <v>6.4590786471211965</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="B34" s="2" t="s">
         <v>0</v>
       </c>
@@ -1092,11 +1687,31 @@
         <v>1.3968316896572641</v>
       </c>
       <c r="F34" s="1">
-        <f>AVERAGE(F21:F32)</f>
-        <v>105.77499999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <f t="shared" ref="F34:K34" si="1">AVERAGE(F21:F32)</f>
+        <v>130.71666666666667</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="1"/>
+        <v>159.5</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="1"/>
+        <v>187.36666666666667</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="1"/>
+        <v>213.25</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="1"/>
+        <v>238.91666666666666</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="1"/>
+        <v>266.41666666666669</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="B35">
         <v>66.515000000000001</v>
       </c>
@@ -1109,7 +1724,7 @@
         <v>105.70753846153845</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:11">
       <c r="B36">
         <v>66.494</v>
       </c>
@@ -1121,7 +1736,7 @@
         <v>77.481142857142842</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:11">
       <c r="B37">
         <v>66.528999999999996</v>
       </c>
@@ -1129,7 +1744,7 @@
         <v>66.72</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:11">
       <c r="B38">
         <v>66.576999999999998</v>
       </c>
@@ -1145,8 +1760,23 @@
       <c r="F38" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="B39">
         <v>66.459999999999994</v>
       </c>
@@ -1160,10 +1790,25 @@
         <v>67.599999999999994</v>
       </c>
       <c r="F39">
-        <v>67.611000000000004</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>68.117999999999995</v>
+      </c>
+      <c r="G39">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H39">
+        <v>69.2</v>
+      </c>
+      <c r="I39">
+        <v>69.7</v>
+      </c>
+      <c r="J39">
+        <v>70.453999999999994</v>
+      </c>
+      <c r="K39">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="B40">
         <v>66.39</v>
       </c>
@@ -1177,10 +1822,25 @@
         <v>67.58</v>
       </c>
       <c r="F40">
-        <v>67.578999999999994</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>68.17</v>
+      </c>
+      <c r="G40">
+        <v>68.7</v>
+      </c>
+      <c r="H40">
+        <v>69.2</v>
+      </c>
+      <c r="I40">
+        <v>69.8</v>
+      </c>
+      <c r="J40">
+        <v>70.543999999999997</v>
+      </c>
+      <c r="K40">
+        <v>71.222999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="B41">
         <v>66.501000000000005</v>
       </c>
@@ -1194,10 +1854,25 @@
         <v>67.599999999999994</v>
       </c>
       <c r="F41">
-        <v>67.635999999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>68</v>
+      </c>
+      <c r="G41">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H41">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="I41">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="J41">
+        <v>70.540000000000006</v>
+      </c>
+      <c r="K41">
+        <v>71.194999999999993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="B42">
         <v>66.52</v>
       </c>
@@ -1211,10 +1886,25 @@
         <v>67.56</v>
       </c>
       <c r="F42">
-        <v>67.656000000000006</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="G42">
+        <v>68.7</v>
+      </c>
+      <c r="H42">
+        <v>69.3</v>
+      </c>
+      <c r="I42">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="J42">
+        <v>70.415999999999997</v>
+      </c>
+      <c r="K42">
+        <v>71.149000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="B43">
         <v>66.525000000000006</v>
       </c>
@@ -1228,10 +1918,25 @@
         <v>67.599999999999994</v>
       </c>
       <c r="F43">
-        <v>67.555000000000007</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>68.12</v>
+      </c>
+      <c r="G43">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H43">
+        <v>69.2</v>
+      </c>
+      <c r="I43">
+        <v>69.8</v>
+      </c>
+      <c r="J43">
+        <v>70.563000000000002</v>
+      </c>
+      <c r="K43">
+        <v>71.162999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -1249,10 +1954,25 @@
         <v>67.5</v>
       </c>
       <c r="F44">
-        <v>67.662000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>68.19</v>
+      </c>
+      <c r="G44">
+        <v>68.7</v>
+      </c>
+      <c r="H44">
+        <v>69.3</v>
+      </c>
+      <c r="I44">
+        <v>69.8</v>
+      </c>
+      <c r="J44">
+        <v>70.588999999999999</v>
+      </c>
+      <c r="K44">
+        <v>71.16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1271,10 +1991,28 @@
         <v>67.599999999999994</v>
       </c>
       <c r="F45">
-        <v>67.67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="G45" s="1">
+        <f>_xlfn.STDEV.S(G39:G44)</f>
+        <v>5.4772255750521283E-2</v>
+      </c>
+      <c r="H45">
+        <v>69.2</v>
+      </c>
+      <c r="I45" s="1">
+        <f>_xlfn.STDEV.S(I39:I44)</f>
+        <v>7.527726527091011E-2</v>
+      </c>
+      <c r="J45" s="1">
+        <f>_xlfn.STDEV.S(J39:J44)</f>
+        <v>6.7417109598876965E-2</v>
+      </c>
+      <c r="K45">
+        <v>71.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="C46" s="1">
         <f>AVERAGE(C37:C44)</f>
         <v>66.778875000000014</v>
@@ -1287,10 +2025,28 @@
       </c>
       <c r="F46" s="1">
         <f>_xlfn.STDEV.S(F39:F45)</f>
-        <v>4.4126441700446779E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>6.1035508790648764E-2</v>
+      </c>
+      <c r="G46" s="1">
+        <f>AVERAGE(G39:G44)</f>
+        <v>68.650000000000006</v>
+      </c>
+      <c r="H46">
+        <v>69.3</v>
+      </c>
+      <c r="I46" s="1">
+        <f>AVERAGE(I39:I44)</f>
+        <v>69.816666666666677</v>
+      </c>
+      <c r="J46" s="1">
+        <f>AVERAGE(J39:J44)</f>
+        <v>70.51766666666667</v>
+      </c>
+      <c r="K46">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
@@ -1303,10 +2059,16 @@
       </c>
       <c r="F47" s="1">
         <f>AVERAGE(F39:F45)</f>
-        <v>67.624142857142857</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>68.114000000000004</v>
+      </c>
+      <c r="H47">
+        <v>69.260000000000005</v>
+      </c>
+      <c r="K47">
+        <v>71.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="B48">
         <v>97.308999999999997</v>
       </c>
@@ -1320,8 +2082,23 @@
       <c r="E48">
         <v>67.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>69.347999999999999</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>71.222999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="B49">
         <v>97.373000000000005</v>
       </c>
@@ -1332,8 +2109,24 @@
         <f>_xlfn.STDEV.S(E39:E48)</f>
         <v>4.5995168828425019E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>98.766999999999996</v>
+      </c>
+      <c r="H49" s="1">
+        <f>_xlfn.STDEV.S(H39:H48)</f>
+        <v>7.1006728945610886E-2</v>
+      </c>
+      <c r="I49">
+        <v>99.9</v>
+      </c>
+      <c r="J49">
+        <v>100.6</v>
+      </c>
+      <c r="K49">
+        <v>71.043999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="B50">
         <v>97.36</v>
       </c>
@@ -1347,8 +2140,25 @@
         <f>AVERAGE(E39:E48)</f>
         <v>67.564000000000007</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>98.68</v>
+      </c>
+      <c r="H50" s="1">
+        <f>AVERAGE(H39:H48)</f>
+        <v>69.270799999999994</v>
+      </c>
+      <c r="I50">
+        <v>100.01</v>
+      </c>
+      <c r="J50">
+        <v>100.58</v>
+      </c>
+      <c r="K50" s="1">
+        <f>_xlfn.STDEV.S(K39:K49)</f>
+        <v>8.5675391608516865E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="B51">
         <v>97.355000000000004</v>
       </c>
@@ -1358,8 +2168,21 @@
       <c r="D51">
         <v>97.48</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51">
+        <v>100</v>
+      </c>
+      <c r="J51">
+        <v>100.672</v>
+      </c>
+      <c r="K51" s="1">
+        <f>AVERAGE(K39:K49)</f>
+        <v>71.141545454545451</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="B52">
         <v>97.394000000000005</v>
       </c>
@@ -1375,8 +2198,20 @@
       <c r="F52" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <v>98.7</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>99.9</v>
+      </c>
+      <c r="J52">
+        <v>100.58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="B53">
         <v>97.331000000000003</v>
       </c>
@@ -1390,10 +2225,25 @@
         <v>97.8</v>
       </c>
       <c r="F53">
-        <v>97.7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>98.162999999999997</v>
+      </c>
+      <c r="G53">
+        <v>98.7</v>
+      </c>
+      <c r="H53">
+        <v>99.4</v>
+      </c>
+      <c r="I53">
+        <v>100</v>
+      </c>
+      <c r="J53">
+        <v>100.718</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1411,10 +2261,25 @@
         <v>97.7</v>
       </c>
       <c r="F54">
-        <v>97.83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>98.245000000000005</v>
+      </c>
+      <c r="G54">
+        <v>98.7</v>
+      </c>
+      <c r="H54">
+        <v>99.34</v>
+      </c>
+      <c r="I54">
+        <v>99.9</v>
+      </c>
+      <c r="J54">
+        <v>100.5</v>
+      </c>
+      <c r="K54">
+        <v>101.46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -1432,10 +2297,26 @@
         <v>97.8</v>
       </c>
       <c r="F55">
-        <v>97.8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>98.21</v>
+      </c>
+      <c r="G55">
+        <v>98.8</v>
+      </c>
+      <c r="H55">
+        <v>99.44</v>
+      </c>
+      <c r="I55" s="1">
+        <f>_xlfn.STDEV.S(I49:I54)</f>
+        <v>5.6715665090576461E-2</v>
+      </c>
+      <c r="J55">
+        <v>100.6</v>
+      </c>
+      <c r="K55">
+        <v>101.241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="C56" s="1">
         <f>_xlfn.STDEV.S(C49:C55)</f>
         <v>3.2423536424725445E-2</v>
@@ -1447,10 +2328,26 @@
         <v>97.85</v>
       </c>
       <c r="F56">
-        <v>97.76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>98.19</v>
+      </c>
+      <c r="G56">
+        <v>98.7</v>
+      </c>
+      <c r="H56">
+        <v>99.33</v>
+      </c>
+      <c r="I56" s="1">
+        <f>AVERAGE(I49:I54)</f>
+        <v>99.951666666666668</v>
+      </c>
+      <c r="J56">
+        <v>100.7</v>
+      </c>
+      <c r="K56">
+        <v>101.411</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="C57" s="1">
         <f>AVERAGE(C49:C55)</f>
         <v>97.319428571428574</v>
@@ -1462,10 +2359,24 @@
         <v>97.73</v>
       </c>
       <c r="F57">
-        <v>97.7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>98.22</v>
+      </c>
+      <c r="G57" s="1">
+        <f>_xlfn.STDEV.S(G49:G56)</f>
+        <v>4.4350873723069874E-2</v>
+      </c>
+      <c r="H57">
+        <v>99.4</v>
+      </c>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3">
+        <v>100.5</v>
+      </c>
+      <c r="K57" s="3">
+        <v>101.232</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="D58">
         <v>97.495999999999995</v>
       </c>
@@ -1474,10 +2385,23 @@
         <v>6.0249481325564305E-2</v>
       </c>
       <c r="F58">
-        <v>97.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>98.22</v>
+      </c>
+      <c r="G58" s="1">
+        <f>AVERAGE(G49:G56)</f>
+        <v>98.721000000000004</v>
+      </c>
+      <c r="H58">
+        <v>99.3</v>
+      </c>
+      <c r="J58" s="3">
+        <v>100.6</v>
+      </c>
+      <c r="K58" s="3">
+        <v>101.43600000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="D59" s="1">
         <f>_xlfn.STDEV.S(D51:D58)</f>
         <v>2.1817014985032444E-2</v>
@@ -1487,23 +2411,99 @@
         <v>97.775999999999996</v>
       </c>
       <c r="F59">
-        <v>97.82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>98.197999999999993</v>
+      </c>
+      <c r="H59">
+        <v>99.4</v>
+      </c>
+      <c r="J59" s="3">
+        <v>100.6</v>
+      </c>
+      <c r="K59" s="3">
+        <v>101.42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="D60" s="1">
         <f>AVERAGE(D51:D58)</f>
         <v>97.481625000000008</v>
       </c>
-      <c r="F60" s="1">
-        <f>_xlfn.STDEV.S(F53:F59)</f>
-        <v>5.4379618030494722E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="F61" s="1">
-        <f>AVERAGE(F53:F59)</f>
-        <v>97.77285714285712</v>
+      <c r="F60">
+        <v>98.21</v>
+      </c>
+      <c r="H60">
+        <v>99.3</v>
+      </c>
+      <c r="J60" s="1">
+        <f>_xlfn.STDEV.S(J49:J59)</f>
+        <v>7.0484556657986142E-2</v>
+      </c>
+      <c r="K60" s="3">
+        <v>101.268</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="F61">
+        <v>98.212000000000003</v>
+      </c>
+      <c r="H61" s="1">
+        <f>_xlfn.STDEV.S(H53:H60)</f>
+        <v>5.2898150116185635E-2</v>
+      </c>
+      <c r="J61" s="1">
+        <f>AVERAGE(J49:J59)</f>
+        <v>100.60454545454546</v>
+      </c>
+      <c r="K61" s="3">
+        <v>101.35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="F62">
+        <v>98.15</v>
+      </c>
+      <c r="H62" s="1">
+        <f>AVERAGE(H53:H60)</f>
+        <v>99.363749999999982</v>
+      </c>
+      <c r="K62" s="3">
+        <v>101.374</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="F63">
+        <v>98.27</v>
+      </c>
+      <c r="K63" s="3">
+        <v>101.264</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="F64">
+        <v>98.28</v>
+      </c>
+      <c r="K64" s="3">
+        <v>101.438</v>
+      </c>
+    </row>
+    <row r="65" spans="6:11">
+      <c r="F65" s="1">
+        <f>_xlfn.STDEV.S(F53:F64)</f>
+        <v>3.824561769310663E-2</v>
+      </c>
+      <c r="K65" s="1">
+        <f>_xlfn.STDEV.S(K54:K64)</f>
+        <v>8.7284591996526703E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="6:11">
+      <c r="F66" s="1">
+        <f>AVERAGE(F53:F64)</f>
+        <v>98.213999999999999</v>
+      </c>
+      <c r="K66" s="1">
+        <f>AVERAGE(K54:K64)</f>
+        <v>101.354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>